<commit_message>
se libera primera version funcional de autogeneracion de casos de borde
</commit_message>
<xml_diff>
--- a/Test/TemplatesTest/WebService1Test/InsertarProducto/InsertarProducto.xlsx
+++ b/Test/TemplatesTest/WebService1Test/InsertarProducto/InsertarProducto.xlsx
@@ -45,9 +45,6 @@
     <t>Caso2</t>
   </si>
   <si>
-    <t>xsd:int</t>
-  </si>
-  <si>
     <t>xsd:decimal</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>DFZBF34457456</t>
+  </si>
+  <si>
+    <t>xsd:integer</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -452,16 +452,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>70</v>
@@ -520,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>1200</v>
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>100</v>

</xml_diff>